<commit_message>
update(results): minor update to results
Signed-off-by: ESCristiano <cris96r@gmail.com>
</commit_message>
<xml_diff>
--- a/results/Availability/000_Intermitent_jul_23/results.xlsx
+++ b/results/Availability/000_Intermitent_jul_23/results.xlsx
@@ -51,7 +51,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -80,12 +80,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -187,7 +181,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -271,7 +265,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -310,6 +304,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -492,11 +487,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="38155551"/>
-        <c:axId val="27389423"/>
+        <c:axId val="45780467"/>
+        <c:axId val="66682706"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="38155551"/>
+        <c:axId val="45780467"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -524,7 +519,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27389423"/>
+        <c:crossAx val="66682706"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -532,7 +527,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="27389423"/>
+        <c:axId val="66682706"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -547,7 +542,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -569,7 +564,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38155551"/>
+        <c:crossAx val="45780467"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -604,13 +599,13 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -628,9 +623,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>578880</xdr:colOff>
+      <xdr:colOff>578520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>27720</xdr:rowOff>
+      <xdr:rowOff>27360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -638,8 +633,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5421600" y="493200"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="5426640" y="493200"/>
+        <a:ext cx="5766840" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -660,10 +655,10 @@
   <dimension ref="B1:O41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24"/>
   </cols>
@@ -704,9 +699,9 @@
       <c r="D3" s="3" t="n">
         <v>608318</v>
       </c>
-      <c r="E3" s="0" t="e">
-        <f aca="false">D3*(1/(1.79769313486232E+308))</f>
-        <v>#VALUE!</v>
+      <c r="E3" s="0" t="n">
+        <f aca="false">D3*(1/(1500000000))</f>
+        <v>0.000405545333333333</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>